<commit_message>
data validation and save $15
</commit_message>
<xml_diff>
--- a/info/bill-of-materials.xlsx
+++ b/info/bill-of-materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattm\Desktop\Coding\hycsg\rocket-radio\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D03447-0660-4DF4-9E8A-D6565ECA30AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF11407-670E-4AC4-9CC6-6D6FDF665B4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16440" yWindow="4785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bill of materials" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -99,6 +99,30 @@
   </si>
   <si>
     <t>https://www.amazon.com/NOYITO-Antenna-Omnidirectional-430-470MHz-Connector/dp/B07J6GYKTZ/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I (Matthew) already have a 5v Arduino Pro Micro that we can use for the ground instead of buying a second 3.3v version (hence the quantity being only 1). The reason for the 3.3v version being necessary for the rocket is that LiPo batteries provide just 3.7v and all the sensors onboard and the radio module are compatible with 3.3v logic.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -108,7 +132,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +271,15 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -604,7 +637,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -615,6 +648,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="16" fillId="30" borderId="5" xfId="39" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="15" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -972,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,14 +1043,14 @@
         <v>4</v>
       </c>
       <c r="B2" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3">
         <v>17.95</v>
       </c>
       <c r="D2" s="3">
         <f t="shared" ref="D2:D10" si="0">B2*C2</f>
-        <v>35.9</v>
+        <v>17.95</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -1169,7 +1205,12 @@
       <c r="C11"/>
       <c r="D11" s="5">
         <f>SUM(D2:D10)</f>
-        <v>88.29</v>
+        <v>70.34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ping test and updated BOM
</commit_message>
<xml_diff>
--- a/info/bill-of-materials.xlsx
+++ b/info/bill-of-materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattm\Desktop\Coding\hycsg\rocket-radio\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF355822-4AA0-48E1-8305-88752FB81263}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C04B32A-52CA-4DC4-A4A9-7468C177E5F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -41,15 +41,9 @@
     <t>100mAh LiPo Battery</t>
   </si>
   <si>
-    <t>MPL3115A2</t>
-  </si>
-  <si>
     <t>Pro Micro 3.3V</t>
   </si>
   <si>
-    <t>LSM6DS33</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
@@ -65,21 +59,12 @@
     <t>https://www.adafruit.com/product/1904</t>
   </si>
   <si>
-    <t>Antenna (optional)</t>
-  </si>
-  <si>
     <t>LiPo Battery Charger</t>
   </si>
   <si>
     <t>https://www.adafruit.com/product/1570</t>
   </si>
   <si>
-    <t>HC-12</t>
-  </si>
-  <si>
-    <t>https://www.banggood.com/custlink/3KGvMGgRvG</t>
-  </si>
-  <si>
     <t>https://www.adafruit.com/product/1769</t>
   </si>
   <si>
@@ -98,31 +83,16 @@
     <t>10x 10u Capacitor (optional, only 2 needed)</t>
   </si>
   <si>
-    <t>https://www.amazon.com/NOYITO-Antenna-Omnidirectional-430-470MHz-Connector/dp/B07J6GYKTZ/</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> I (Matthew) already have a 5v Arduino Pro Micro that we can use for the ground instead of buying a second 3.3v version (hence the quantity being only 1). The reason for the 3.3v version being necessary for the rocket is that LiPo batteries provide just 3.7v and all the sensors onboard and the radio module are compatible with 3.3v logic.</t>
-    </r>
+    <t>https://www.adafruit.com/product/3073</t>
+  </si>
+  <si>
+    <t>MPL3115A2 Breakout</t>
+  </si>
+  <si>
+    <t>LSM6DS33 Breakout</t>
+  </si>
+  <si>
+    <t>LoRa Radio Transceiver Breakout</t>
   </si>
 </sst>
 </file>
@@ -132,7 +102,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,15 +241,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -637,7 +598,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -648,9 +609,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="16" fillId="30" borderId="5" xfId="39" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="15" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1011,7 +969,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E9" sqref="E8:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,18 +987,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -1053,12 +1011,12 @@
         <v>17.95</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -1071,12 +1029,12 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
@@ -1089,25 +1047,25 @@
         <v>5.95</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
       </c>
       <c r="C5" s="3">
-        <v>6.95</v>
+        <v>19.95</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" si="0"/>
-        <v>13.9</v>
+        <v>39.9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1125,12 +1083,12 @@
         <v>5.95</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -1143,12 +1101,12 @@
         <v>6.95</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
@@ -1161,12 +1119,12 @@
         <v>0.75</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
@@ -1179,53 +1137,34 @@
         <v>1.95</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3">
-        <v>6.99</v>
-      </c>
-      <c r="D10" s="3">
-        <f t="shared" si="0"/>
-        <v>6.99</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="5">
+        <f>SUM(D2:D9)</f>
+        <v>89.350000000000009</v>
+      </c>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11"/>
       <c r="C11"/>
-      <c r="D11" s="5">
-        <f>SUM(D2:D10)</f>
-        <v>70.34</v>
-      </c>
     </row>
-    <row r="13" spans="1:5" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{02A54F92-1C1E-42BB-B26F-310D0FCF9749}"/>
     <hyperlink ref="E4" r:id="rId2" xr:uid="{5752F5CA-623D-4D79-A2E4-E3540F71D363}"/>
     <hyperlink ref="E3" r:id="rId3" xr:uid="{E2FC6238-FA2B-4FF8-87BF-872ED371C41E}"/>
     <hyperlink ref="E7" r:id="rId4" xr:uid="{03408FE2-A415-4D46-B399-184932E0C3B4}"/>
-    <hyperlink ref="E10" r:id="rId5" xr:uid="{2C98DDF7-B0DC-423D-8FA8-9C8DFC81443F}"/>
-    <hyperlink ref="E6" r:id="rId6" xr:uid="{87C244FE-8A04-473C-9217-440DC5FC94C8}"/>
-    <hyperlink ref="E5" r:id="rId7" xr:uid="{E1676BD2-F45D-4836-9FEE-3839C98C5E83}"/>
-    <hyperlink ref="E8" r:id="rId8" xr:uid="{E10DC99A-0812-4B9E-AA61-9B370175CB37}"/>
-    <hyperlink ref="E9" r:id="rId9" xr:uid="{7F30F969-9F77-4363-B0FE-71FFEE4EE573}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{87C244FE-8A04-473C-9217-440DC5FC94C8}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{E1676BD2-F45D-4836-9FEE-3839C98C5E83}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{E10DC99A-0812-4B9E-AA61-9B370175CB37}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{7F30F969-9F77-4363-B0FE-71FFEE4EE573}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>